<commit_message>
chore: Clean SP values columns and update value verification logic
</commit_message>
<xml_diff>
--- a/input_data/data_errors_03/valores.xlsx
+++ b/input_data/data_errors_03/valores.xlsx
@@ -426,14 +426,15 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="24.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="3" style="3" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>